<commit_message>
Cleaned APIs code and updated error messages
</commit_message>
<xml_diff>
--- a/Burger and Fries.xlsx
+++ b/Burger and Fries.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code Space\projects\burger-and-fries\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41680D3-8DE3-4FD7-82C2-73C19BE57724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>Requirement</t>
   </si>
@@ -43,14 +49,37 @@
     <t>HTTP Status code</t>
   </si>
   <si>
-    <t>Create try catch block for every api</t>
+    <t>Create CRUD API for food categories</t>
+  </si>
+  <si>
+    <t>categoryController.js</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>Change category field of product.model to the reference of category.model</t>
+  </si>
+  <si>
+    <t>productController.js &amp; product.model</t>
+  </si>
+  <si>
+    <t>Clean code over all</t>
+  </si>
+  <si>
+    <t>Draw block diagram of req, res cycle as per my understandng</t>
+  </si>
+  <si>
+    <t>Checkout NoSQL booster</t>
+  </si>
+  <si>
+    <t>Add pagination to getProducts API of productController.js</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -73,12 +102,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -100,32 +135,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -136,10 +177,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -177,71 +218,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -269,7 +310,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -292,11 +333,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -305,13 +346,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -321,7 +362,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -330,7 +371,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -339,7 +380,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -347,10 +388,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -415,31 +456,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="48.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="32.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="62.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20" style="1" customWidth="1"/>
+    <col min="3" max="4" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -463,19 +499,23 @@
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
+      <c r="C2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -483,19 +523,21 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="32.25" customFormat="1" s="1">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="C3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="4"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -503,15 +545,19 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:12" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="B4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -519,13 +565,19 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -533,13 +585,19 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+    <row r="6" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -547,13 +605,17 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+    <row r="7" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -561,13 +623,15 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+    <row r="8" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -575,13 +639,17 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+    <row r="9" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -589,13 +657,13 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+    <row r="10" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -603,13 +671,13 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+    <row r="11" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -617,13 +685,13 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+    <row r="12" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -631,13 +699,13 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+    <row r="13" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -645,13 +713,13 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+    <row r="14" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -659,13 +727,13 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+    <row r="15" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -673,13 +741,13 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+    <row r="16" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -687,13 +755,13 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+    <row r="17" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -701,13 +769,13 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+    <row r="18" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -715,13 +783,13 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+    <row r="19" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -729,13 +797,13 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+    <row r="20" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -743,13 +811,13 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+    <row r="21" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
@@ -757,13 +825,13 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+    <row r="22" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
@@ -771,13 +839,13 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
+    <row r="23" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
@@ -785,13 +853,13 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
+    <row r="24" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
@@ -799,13 +867,13 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
+    <row r="25" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
@@ -813,13 +881,13 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
+    <row r="26" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
@@ -827,13 +895,13 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+    <row r="27" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
@@ -841,13 +909,13 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
+    <row r="28" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
@@ -855,6 +923,30 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Applied json validation to addProduct API request body
</commit_message>
<xml_diff>
--- a/Burger and Fries.xlsx
+++ b/Burger and Fries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code Space\projects\burger-and-fries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41680D3-8DE3-4FD7-82C2-73C19BE57724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F32CAE4-3D53-4CA8-B2A7-B649AB6BC93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Requirement</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t>Add pagination to getProducts API of productController.js</t>
+  </si>
+  <si>
+    <t>JSON Schema validator</t>
+  </si>
+  <si>
+    <t>vs code extension : code spell checker</t>
   </si>
 </sst>
 </file>
@@ -463,7 +469,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection sqref="A1:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,7 +562,9 @@
         <v>11</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="F4" s="4"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -585,16 +593,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>11</v>
-      </c>
+    <row r="6" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -605,11 +604,13 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="C7" s="5" t="s">
         <v>11</v>
       </c>
@@ -625,10 +626,12 @@
     </row>
     <row r="8" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="4"/>
+      <c r="C8" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -641,12 +644,12 @@
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="4"/>
+        <v>16</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -658,9 +661,15 @@
       <c r="L9" s="3"/>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="4"/>
+      <c r="A10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -686,7 +695,9 @@
       <c r="L11" s="3"/>
     </row>
     <row r="12" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+      <c r="A12" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="B12" s="6"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -949,5 +960,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>